<commit_message>
[Add] 몬스터 Projectile 생성
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excels/MonsterSheets.xlsx
+++ b/Assets/Resources/Excels/MonsterSheets.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sparta_team\3D_TEAM12\Assets\Resources\Excels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCBE4F1-CBAF-493E-9251-C113A6EAB9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48315" yWindow="2820" windowWidth="19335" windowHeight="15285"/>
+    <workbookView xWindow="56295" yWindow="3345" windowWidth="20505" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterList" sheetId="2" r:id="rId1"/>
     <sheet name="SkillList" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,13 +139,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Prefabs/Projectiles/Monster/SkeletonMinion_Default</t>
-  </si>
-  <si>
-    <t>/Prefabs/Projectiles/Monster/SkeletonMinion_Default</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스켈레톤 로그</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,10 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Prefabs/Projectiles/Monster/SkeletonMinion_Default</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>스켈레톤 레인저</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -202,13 +197,40 @@
   <si>
     <t>/Prefabs/Monsters/Skeleton_Giant</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>startScale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>endScale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waitTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>knockbackPower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>knockbackDuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Projectiles/Monster/SkeletonMinion_Default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,38 +540,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.58203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13.375" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
     <col min="10" max="10" width="6.5" customWidth="1"/>
-    <col min="11" max="11" width="5.625" customWidth="1"/>
+    <col min="11" max="11" width="5.58203125" customWidth="1"/>
     <col min="12" max="12" width="10.75" customWidth="1"/>
-    <col min="13" max="13" width="14.125" customWidth="1"/>
+    <col min="13" max="13" width="14.08203125" customWidth="1"/>
     <col min="14" max="14" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="15" max="15" width="11.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -643,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -657,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -690,21 +712,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>10003</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
@@ -737,21 +759,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>10004</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
@@ -784,21 +806,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>10005</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -831,21 +853,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>10006</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -878,18 +900,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>10007</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
         <v>26</v>
@@ -929,24 +951,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.375" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -965,13 +990,34 @@
       <c r="F1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>10001</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -985,13 +1031,34 @@
       <c r="F2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>10002</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1005,13 +1072,34 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>0.4</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>10002</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>0.3</v>
@@ -1025,13 +1113,34 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0.4</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>10003</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1045,13 +1154,34 @@
       <c r="F5">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>10003</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>0.8</v>
@@ -1065,13 +1195,34 @@
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>0.4</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>10004</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1085,13 +1236,34 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>0.4</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>10005</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1105,13 +1277,34 @@
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>10006</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1125,13 +1318,34 @@
       <c r="F9">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0.4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>10006</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1145,13 +1359,34 @@
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>0.4</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10006</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>0.5</v>
@@ -1165,13 +1400,34 @@
       <c r="F11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>0.4</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10007</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1185,13 +1441,34 @@
       <c r="F12">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>0.4</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>10007</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1204,10 +1481,32 @@
       </c>
       <c r="F13">
         <v>2.5</v>
+      </c>
+      <c r="G13">
+        <v>0.4</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Fix] Projectile 오류 수정
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excels/MonsterSheets.xlsx
+++ b/Assets/Resources/Excels/MonsterSheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\sparta_team\3D_TEAM12\Assets\Resources\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E75C3D9-DC0C-4FB4-843D-349F11C435E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30CBE9A-18F2-46B7-BE57-DEA8D523A18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52770" yWindow="2640" windowWidth="20505" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53160" yWindow="2535" windowWidth="20520" windowHeight="15285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterList" sheetId="2" r:id="rId1"/>
@@ -234,14 +234,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/Projectiles/Monster/MeleeAttack</t>
-  </si>
-  <si>
-    <t>/Projectiles/Monster/Fireball</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/Projectiles/Monster/Arrow</t>
+    <t>/Projectiles/Monster/Monster_MeleeAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Projectiles/Monster/Monster_Fireball</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/Projectiles/Monster/Monster_Arrow</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -974,7 +975,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>